<commit_message>
fix 400 error handle
</commit_message>
<xml_diff>
--- a/seo_report_2025-11-23.xlsx
+++ b/seo_report_2025-11-23.xlsx
@@ -589,25 +589,17 @@
           <t>SÍ</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="L2" s="2" t="n">
+        <v>96</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -666,25 +658,17 @@
           <t>SÍ</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="L3" s="2" t="n">
+        <v>96</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="4">
@@ -743,25 +727,17 @@
           <t>SÍ</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="L4" s="2" t="n">
+        <v>96</v>
+      </c>
+      <c r="M4" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="5">
@@ -820,15 +796,11 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="L5" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>91</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -897,15 +869,11 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="L6" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>91</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -974,15 +942,11 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="L7" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>91</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -1282,25 +1246,17 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="L11" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="M11" s="2" t="n">
+        <v>97</v>
+      </c>
+      <c r="N11" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="O11" s="2" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="12">
@@ -1359,25 +1315,17 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="L12" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="M12" s="2" t="n">
+        <v>97</v>
+      </c>
+      <c r="N12" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="O12" s="2" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="13">
@@ -1436,25 +1384,17 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="L13" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="M13" s="2" t="n">
+        <v>97</v>
+      </c>
+      <c r="N13" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="O13" s="2" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="14">
@@ -1513,25 +1453,17 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="L14" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="M14" s="2" t="n">
+        <v>98</v>
+      </c>
+      <c r="N14" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="O14" s="2" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="15">
@@ -1590,25 +1522,17 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="L15" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="M15" s="2" t="n">
+        <v>98</v>
+      </c>
+      <c r="N15" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="O15" s="2" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="16">
@@ -1667,25 +1591,17 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="L16" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="M16" s="2" t="n">
+        <v>98</v>
+      </c>
+      <c r="N16" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="O16" s="2" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="17">
@@ -1744,25 +1660,17 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="L17" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="M17" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="N17" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="O17" s="2" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="18">
@@ -1778,27 +1686,27 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Anuncios Clasificados Bolivia | Escorts, Masajes y Acompañantes | Damas de Compañía Bolivia</t>
-        </is>
-      </c>
-      <c r="D18" s="2" t="inlineStr">
-        <is>
-          <t>SÍ</t>
+          <t>ERROR</t>
+        </is>
+      </c>
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Encuentra anuncios clasificados para adultos en Bolivia. Escorts verificadas, masajes, acompañantes en La Paz, Santa Cruz, Cochabamba. Contacto directo por WhatsApp.</t>
-        </is>
-      </c>
-      <c r="F18" s="2" t="inlineStr">
-        <is>
-          <t>SÍ</t>
+          <t>ERROR</t>
+        </is>
+      </c>
+      <c r="F18" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Anuncios en Bolivia</t>
+          <t>ERROR</t>
         </is>
       </c>
       <c r="H18" s="3" t="inlineStr">
@@ -1808,12 +1716,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>BLANQUITAMACANUDATETONASALIDAS pechitos naturales | JOVENCITA ARDIENTE LISTA PARA HACER REALIDAD TUS FANTASIAS MAS CALIENTES | MANANEAMOS BABY | exclusiva paraguaya trato sin complicaciones mis fotos son 100 reales y tengo lugar propio | LINDA CULONA SERVICIO SIN COMPLICACIONES AMOR TE HARE UN BUEN ORAL BEBE ESCRIBEME Y LLEGAMOS A UN BUEN TRATO TRATO | Luxury Spa | Macanuda nalgona | Masajes Relajantes y Sensuales Exclusivo Para Caballeros | Morena linda delgada hago de todo y soy muy sociable | Nicky iniciante</t>
-        </is>
-      </c>
-      <c r="J18" s="3" t="inlineStr">
-        <is>
-          <t>0 de 10</t>
+          <t>ERROR</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>0 de 0</t>
         </is>
       </c>
       <c r="K18" s="3" t="inlineStr">
@@ -1821,25 +1729,17 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="L18" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="M18" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="N18" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="O18" s="2" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="19">
@@ -1855,7 +1755,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Anuncios Clasificados Bolivia | Escorts, Masajes y Acompañantes | Damas de Compañía Bolivia</t>
+          <t>ERROR</t>
         </is>
       </c>
       <c r="D19" s="3" t="inlineStr">
@@ -1865,7 +1765,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Encuentra anuncios clasificados para adultos en Bolivia. Escorts verificadas, masajes, acompañantes en La Paz, Santa Cruz, Cochabamba. Contacto directo por WhatsApp.</t>
+          <t>ERROR</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
@@ -1875,7 +1775,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Anuncios en Bolivia</t>
+          <t>ERROR</t>
         </is>
       </c>
       <c r="H19" s="3" t="inlineStr">
@@ -1885,12 +1785,12 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>BLANQUITAMACANUDATETONASALIDAS pechitos naturales | JOVENCITA ARDIENTE LISTA PARA HACER REALIDAD TUS FANTASIAS MAS CALIENTES | MANANEAMOS BABY | exclusiva paraguaya trato sin complicaciones mis fotos son 100 reales y tengo lugar propio | LINDA CULONA SERVICIO SIN COMPLICACIONES AMOR TE HARE UN BUEN ORAL BEBE ESCRIBEME Y LLEGAMOS A UN BUEN TRATO TRATO | Luxury Spa | Macanuda nalgona | Masajes Relajantes y Sensuales Exclusivo Para Caballeros | Morena linda delgada hago de todo y soy muy sociable | Nicky iniciante</t>
-        </is>
-      </c>
-      <c r="J19" s="3" t="inlineStr">
-        <is>
-          <t>0 de 10</t>
+          <t>ERROR</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>0 de 0</t>
         </is>
       </c>
       <c r="K19" s="3" t="inlineStr">
@@ -1898,25 +1798,17 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="L19" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="M19" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="N19" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="O19" s="2" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="20">
@@ -1932,17 +1824,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Anuncios Clasificados Bolivia | Escorts, Masajes y Acompañantes | Damas de Compañía Bolivia</t>
-        </is>
-      </c>
-      <c r="D20" s="2" t="inlineStr">
-        <is>
-          <t>SÍ</t>
+          <t>ERROR</t>
+        </is>
+      </c>
+      <c r="D20" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Encuentra anuncios clasificados para adultos en Bolivia. Escorts verificadas, masajes, acompañantes en La Paz, Santa Cruz, Cochabamba. Contacto directo por WhatsApp.</t>
+          <t>ERROR</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
@@ -1952,7 +1844,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Anuncios en Bolivia</t>
+          <t>ERROR</t>
         </is>
       </c>
       <c r="H20" s="3" t="inlineStr">
@@ -1962,12 +1854,12 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>19 Años TATIANA | holi recien estoy empezando en esto | Hoy te traigo un buen contenido no te lo pierdas | INICIANTE 20 ANITOS | LAU Tu flaquita rica y apretadita Pura dinamita en un cuerpo pequeno Listo para la explosion | Llegue de viaje soy una damita de piel canela atenta y muy tierna | MARIBEL 19 Años TU NOVIA VIPFOTO REAL | FLAQUITA BONITA CACHONDA NUEVA EN EL AMBIENTE</t>
-        </is>
-      </c>
-      <c r="J20" s="3" t="inlineStr">
-        <is>
-          <t>0 de 8</t>
+          <t>ERROR</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>0 de 0</t>
         </is>
       </c>
       <c r="K20" s="3" t="inlineStr">
@@ -2009,27 +1901,27 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Anuncios Clasificados Bolivia | Escorts, Masajes y Acompañantes | Damas de Compañía Bolivia</t>
-        </is>
-      </c>
-      <c r="D21" s="2" t="inlineStr">
-        <is>
-          <t>SÍ</t>
+          <t>ERROR</t>
+        </is>
+      </c>
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Encuentra anuncios clasificados para adultos en Bolivia. Escorts verificadas, masajes, acompañantes en La Paz, Santa Cruz, Cochabamba. Contacto directo por WhatsApp.</t>
-        </is>
-      </c>
-      <c r="F21" s="2" t="inlineStr">
-        <is>
-          <t>SÍ</t>
+          <t>ERROR</t>
+        </is>
+      </c>
+      <c r="F21" s="3" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Anuncios en Bolivia</t>
+          <t>ERROR</t>
         </is>
       </c>
       <c r="H21" s="3" t="inlineStr">
@@ -2039,12 +1931,12 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>19 Años TATIANA | holi recien estoy empezando en esto | Hoy te traigo un buen contenido no te lo pierdas | INICIANTE 20 ANITOS | LAU Tu flaquita rica y apretadita Pura dinamita en un cuerpo pequeno Listo para la explosion | Llegue de viaje soy una damita de piel canela atenta y muy tierna | MARIBEL 19 Años TU NOVIA VIPFOTO REAL | FLAQUITA BONITA CACHONDA NUEVA EN EL AMBIENTE</t>
-        </is>
-      </c>
-      <c r="J21" s="3" t="inlineStr">
-        <is>
-          <t>0 de 8</t>
+          <t>ERROR</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>0 de 0</t>
         </is>
       </c>
       <c r="K21" s="3" t="inlineStr">
@@ -2086,7 +1978,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Anuncios Clasificados Bolivia | Escorts, Masajes y Acompañantes | Damas de Compañía Bolivia</t>
+          <t>ERROR</t>
         </is>
       </c>
       <c r="D22" s="3" t="inlineStr">
@@ -2096,7 +1988,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Encuentra anuncios clasificados para adultos en Bolivia. Escorts verificadas, masajes, acompañantes en La Paz, Santa Cruz, Cochabamba. Contacto directo por WhatsApp.</t>
+          <t>ERROR</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
@@ -2106,7 +1998,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Anuncios en Bolivia</t>
+          <t>ERROR</t>
         </is>
       </c>
       <c r="H22" s="3" t="inlineStr">
@@ -2116,12 +2008,12 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>19 Años TATIANA | holi recien estoy empezando en esto | Hoy te traigo un buen contenido no te lo pierdas | INICIANTE 20 ANITOS | LAU Tu flaquita rica y apretadita Pura dinamita en un cuerpo pequeno Listo para la explosion | Llegue de viaje soy una damita de piel canela atenta y muy tierna | MARIBEL 19 Años TU NOVIA VIPFOTO REAL | FLAQUITA BONITA CACHONDA NUEVA EN EL AMBIENTE</t>
-        </is>
-      </c>
-      <c r="J22" s="3" t="inlineStr">
-        <is>
-          <t>0 de 8</t>
+          <t>ERROR</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>0 de 0</t>
         </is>
       </c>
       <c r="K22" s="3" t="inlineStr">

</xml_diff>